<commit_message>
add gasoline and transger to email api
</commit_message>
<xml_diff>
--- a/Data/Finances - Copy.xlsx
+++ b/Data/Finances - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Expenses!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Gasoline!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Incomes!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time History'!$A$1:$C$8</definedName>
   </definedNames>
@@ -1237,7 +1238,8 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,8 +1367,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:E47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,8 +2323,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,7 +2830,8 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,6 +2874,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>